<commit_message>
Concertando a modelagem do banco
</commit_message>
<xml_diff>
--- a/documentacao/product-backlog-ubaturismo.xlsx
+++ b/documentacao/product-backlog-ubaturismo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\FACULDADE\PROJETO INDIVIDUAL\Ubaturismo\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3B3073E-3897-46FC-8908-05D47A07B6B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C787CC3C-B81A-41D3-B145-4DABD79D0A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{25E88591-A2CB-4B21-B72E-E8A51CC9401C}"/>
   </bookViews>
@@ -231,7 +231,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,13 +246,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="36"/>
-      <color theme="1"/>
-      <name val="Aptos Black"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -317,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -335,15 +328,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -430,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,63 +428,60 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -841,7 +822,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,34 +845,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="N2" s="11"/>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
@@ -978,19 +949,19 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="20" t="s">
+      <c r="E7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1105,19 +1076,19 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="20" t="s">
+      <c r="E14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1145,7 +1116,7 @@
       <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="4" t="s">
         <v>51</v>
       </c>
@@ -1167,7 +1138,7 @@
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>53</v>
       </c>
@@ -1189,7 +1160,7 @@
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="4" t="s">
         <v>56</v>
       </c>
@@ -1207,7 +1178,7 @@
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="4" t="s">
         <v>58</v>
       </c>
@@ -1225,7 +1196,7 @@
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="22"/>
       <c r="C20" s="4" t="s">
         <v>59</v>
       </c>

</xml_diff>